<commit_message>
chage columns names in test.xlsx
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>b2</t>
   </si>
@@ -36,15 +36,6 @@
     <t>c3</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>a4</t>
   </si>
   <si>
@@ -61,6 +52,12 @@
   </si>
   <si>
     <t>c5</t>
+  </si>
+  <si>
+    <t>hhhh</t>
+  </si>
+  <si>
+    <t>nnnn</t>
   </si>
 </sst>
 </file>
@@ -405,23 +402,23 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>6</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>6666</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -432,7 +429,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -443,26 +440,26 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -476,7 +473,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -488,7 +485,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>